<commit_message>
[Anuj] Master Branch. Mades changes to Exception handling flow in UC3 and UC4
</commit_message>
<xml_diff>
--- a/BookTable_1.xlsx
+++ b/BookTable_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajay Sharma\Documents\UiPath\BooksWagon Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4373827-F4E5-4C02-9CE0-1D560355DCBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E356F-61C1-48F9-A031-2A571E2112B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="390" windowWidth="12675" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="390" windowWidth="17655" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
[Anuj].Refactor Added Extra Business Exception handling cases
</commit_message>
<xml_diff>
--- a/BookTable_1.xlsx
+++ b/BookTable_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajay Sharma\Documents\UiPath\BooksWagon Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E356F-61C1-48F9-A031-2A571E2112B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DBFF17-4380-4795-AA77-3D07957F8A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="390" windowWidth="17655" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,14 +36,14 @@
     <t>BookDescription</t>
   </si>
   <si>
-    <t>Secret Ruby</t>
+    <t>Circles of Hell</t>
   </si>
   <si>
     <t xml:space="preserve">_x000D_
-By: Imogen White (Author) Usborne Publishing Ltd 2018 </t>
-  </si>
-  <si>
-    <t>Rs.480</t>
+By: Au (Author) , Dante (Author) Penguin Books Ltd 2015 </t>
+  </si>
+  <si>
+    <t>Rs.49</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
[Anuj] Refactor. Added changes to Scraping workflow
</commit_message>
<xml_diff>
--- a/BookTable_1.xlsx
+++ b/BookTable_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajay Sharma\Documents\UiPath\BooksWagon Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DBFF17-4380-4795-AA77-3D07957F8A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA123B7B-2B77-4F62-861D-E27098F44298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="390" windowWidth="17655" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="1485" windowWidth="17655" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>BookPrice</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>BookDescription</t>
+  </si>
+  <si>
+    <t>Harry Potter - Creatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_x000D_
+By: Warner Bros. | (Author) , Bros (Author) Bloomsbury Publishing PLC _x000D_
+Released: 01 Nov 2018 </t>
+  </si>
+  <si>
+    <t>Rs.620</t>
+  </si>
+  <si>
+    <t>Ruby in the Smoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_x000D_
+Scholastic 2015 </t>
+  </si>
+  <si>
+    <t>Rs.237</t>
   </si>
   <si>
     <t>Circles of Hell</t>
@@ -365,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -389,7 +410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -398,6 +419,28 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>